<commit_message>
Nathan's hours week 3
</commit_message>
<xml_diff>
--- a/booked_hours_individual/Booked_Hours_NathanONeill.xlsx
+++ b/booked_hours_individual/Booked_Hours_NathanONeill.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/23206294_student_uwa_edu_au/Documents/CITS3200/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:40009_{3CF58E6A-5DF7-4373-BB5C-FF4A4CCF2CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{054A1911-9F01-49D2-99A2-0BEA2C6957AC}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:40009_{3CF58E6A-5DF7-4373-BB5C-FF4A4CCF2CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{650621C6-2C58-45A3-AC14-70BE0756C40F}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
   <si>
     <t>Wk</t>
   </si>
@@ -63,8 +63,32 @@
 Hours</t>
   </si>
   <si>
+    <t>Created team group, contacted members and conducted background research</t>
+  </si>
+  <si>
+    <t>Initial client meeting with Mrs Caruso</t>
+  </si>
+  <si>
+    <t>Researching skills and resources</t>
+  </si>
+  <si>
+    <t>First online meeting with group members</t>
+  </si>
+  <si>
+    <t>Formal meeting</t>
+  </si>
+  <si>
+    <t>Preparing skills and resources audit deliverable</t>
+  </si>
+  <si>
+    <t>Researching audio similarity software/libraries &amp; implementation of scoring metrics</t>
+  </si>
+  <si>
+    <t>Corresponding with Mr Wise</t>
+  </si>
+  <si>
     <r>
-      <t>CITS3200 Project Billed Hours Record for NathanO'Neill</t>
+      <t>CITS3200 Project Billed Hours Record for Nathan O'Neill</t>
     </r>
     <r>
       <rPr>
@@ -75,24 +99,12 @@
 Each time you do some work on the project, note the week number, start and end date and hour, plus a brief description of the activity. At the end of each week send a copy of the sheet as it currently stands to your group's manager for recording on the group TimeSheet. Date in the form DD/MM/YY and time as XX:YY (24hr clock)</t>
     </r>
   </si>
-  <si>
-    <t>Created team group, contacted members and conducted background research</t>
-  </si>
-  <si>
-    <t>Initial client meeting with Mrs Caruso</t>
-  </si>
-  <si>
-    <t>First meeting with group members</t>
-  </si>
-  <si>
-    <t>Researching skills and resources</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -114,6 +126,11 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -276,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -348,6 +365,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,10 +470,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -763,7 +797,7 @@
   <dimension ref="A1:I132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -782,7 +816,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -836,20 +870,20 @@
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="20">
         <v>43671</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="21">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="20">
         <v>43671</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="21">
         <v>0.45833333333333331</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="6">
         <f>IF(I4&gt;0,I4,IF(I4=0, " ", "ERROR"))</f>
@@ -868,20 +902,20 @@
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="20">
         <v>43679</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="21">
         <v>0.375</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="20">
         <v>43679</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="21">
         <v>0.39583333333333331</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" s="6">
         <f>IF(I5&gt;0,I5,IF(I5=0, " ", "ERROR"))</f>
@@ -900,23 +934,23 @@
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="20">
         <v>43679</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="21">
         <v>0.39583333333333331</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="20">
         <v>43679</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="21">
         <v>0.41666666666666669</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="6">
-        <f t="shared" ref="G5:G30" si="1">IF(I6&gt;0,I6,IF(I6=0, " ", "ERROR"))</f>
+        <f t="shared" ref="G6:G30" si="1">IF(I6&gt;0,I6,IF(I6=0, " ", "ERROR"))</f>
         <v>0.49999999988358468</v>
       </c>
       <c r="H6" s="1">
@@ -932,20 +966,20 @@
       <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="20">
         <v>43681</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="21">
         <v>0.75</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="20">
         <v>43681</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="21">
         <v>0.79166666666666663</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="1"/>
@@ -961,75 +995,131 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
-      <c r="G8" s="6" t="str">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="20">
+        <v>43683</v>
+      </c>
+      <c r="C8" s="23">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D8" s="24">
+        <v>43683</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H8" s="1" t="str">
+        <v>1.3333333333139308</v>
+      </c>
+      <c r="H8" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>4.3333333333139308</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.3333333333139308</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
-      <c r="G9" s="6" t="str">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="24">
+        <v>43685</v>
+      </c>
+      <c r="C9" s="21">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D9" s="24">
+        <v>43685</v>
+      </c>
+      <c r="E9" s="21">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H9" s="1" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="H9" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>5.8333333333139308</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5"/>
-      <c r="G10" s="6" t="str">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="20">
+        <v>43656</v>
+      </c>
+      <c r="C10" s="21">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D10" s="20">
+        <v>43656</v>
+      </c>
+      <c r="E10" s="21">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H10" s="1" t="str">
+        <v>0.16666666668606922</v>
+      </c>
+      <c r="H10" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>6</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16666666668606922</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
-      <c r="G11" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H11" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+      <c r="A11" s="19">
+        <v>3</v>
+      </c>
+      <c r="B11" s="20">
+        <v>43656</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D11" s="20">
+        <v>43656</v>
+      </c>
+      <c r="E11" s="21">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="22">
+        <f t="shared" ref="G11" si="3">IF(I11&gt;0,I11,IF(I11=0, " ", "ERROR"))</f>
+        <v>1.5</v>
+      </c>
+      <c r="H11" s="19">
+        <f t="shared" ref="H11" si="4">IF(AND(G11&lt;&gt;" ",G11&lt;&gt;"ERROR",H10&lt;&gt;" ", H10&lt;&gt;"ERROR"),G11+H10," ")</f>
+        <v>7.5</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1428,7 +1518,7 @@
       <c r="D33" s="4"/>
       <c r="E33" s="5"/>
       <c r="G33" s="6" t="str">
-        <f t="shared" ref="G33:G64" si="3">IF(I33&gt;0,I33,IF(I33=0, " ", "ERROR"))</f>
+        <f t="shared" ref="G33:G64" si="5">IF(I33&gt;0,I33,IF(I33=0, " ", "ERROR"))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H33" s="1" t="str">
@@ -1446,11 +1536,11 @@
       <c r="D34" s="4"/>
       <c r="E34" s="5"/>
       <c r="G34" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H34" s="1" t="str">
-        <f t="shared" ref="H34:H64" si="4">IF(AND(G34&lt;&gt;" ",G34&lt;&gt;"ERROR",H33&lt;&gt;" ", H33&lt;&gt;"ERROR"),G34+H33," ")</f>
+        <f t="shared" ref="H34:H64" si="6">IF(AND(G34&lt;&gt;" ",G34&lt;&gt;"ERROR",H33&lt;&gt;" ", H33&lt;&gt;"ERROR"),G34+H33," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I34" s="1">
@@ -1464,11 +1554,11 @@
       <c r="D35" s="4"/>
       <c r="E35" s="5"/>
       <c r="G35" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H35" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I35" s="1">
@@ -1482,11 +1572,11 @@
       <c r="D36" s="4"/>
       <c r="E36" s="5"/>
       <c r="G36" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H36" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I36" s="1">
@@ -1500,11 +1590,11 @@
       <c r="D37" s="4"/>
       <c r="E37" s="5"/>
       <c r="G37" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H37" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I37" s="1">
@@ -1518,11 +1608,11 @@
       <c r="D38" s="4"/>
       <c r="E38" s="5"/>
       <c r="G38" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H38" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I38" s="1">
@@ -1536,11 +1626,11 @@
       <c r="D39" s="4"/>
       <c r="E39" s="5"/>
       <c r="G39" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H39" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I39" s="1">
@@ -1554,11 +1644,11 @@
       <c r="D40" s="4"/>
       <c r="E40" s="5"/>
       <c r="G40" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H40" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I40" s="1">
@@ -1572,11 +1662,11 @@
       <c r="D41" s="4"/>
       <c r="E41" s="5"/>
       <c r="G41" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H41" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I41" s="1">
@@ -1590,11 +1680,11 @@
       <c r="D42" s="4"/>
       <c r="E42" s="5"/>
       <c r="G42" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H42" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I42" s="1">
@@ -1608,11 +1698,11 @@
       <c r="D43" s="4"/>
       <c r="E43" s="5"/>
       <c r="G43" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H43" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I43" s="1">
@@ -1626,11 +1716,11 @@
       <c r="D44" s="4"/>
       <c r="E44" s="5"/>
       <c r="G44" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H44" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I44" s="1">
@@ -1644,11 +1734,11 @@
       <c r="D45" s="4"/>
       <c r="E45" s="5"/>
       <c r="G45" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H45" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I45" s="1">
@@ -1662,11 +1752,11 @@
       <c r="D46" s="4"/>
       <c r="E46" s="5"/>
       <c r="G46" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H46" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I46" s="1">
@@ -1680,11 +1770,11 @@
       <c r="D47" s="4"/>
       <c r="E47" s="5"/>
       <c r="G47" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H47" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I47" s="1">
@@ -1698,11 +1788,11 @@
       <c r="D48" s="4"/>
       <c r="E48" s="5"/>
       <c r="G48" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H48" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I48" s="1">
@@ -1716,11 +1806,11 @@
       <c r="D49" s="4"/>
       <c r="E49" s="5"/>
       <c r="G49" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H49" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I49" s="1">
@@ -1734,11 +1824,11 @@
       <c r="D50" s="4"/>
       <c r="E50" s="5"/>
       <c r="G50" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H50" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I50" s="1">
@@ -1752,11 +1842,11 @@
       <c r="D51" s="4"/>
       <c r="E51" s="5"/>
       <c r="G51" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H51" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I51" s="1">
@@ -1770,11 +1860,11 @@
       <c r="D52" s="4"/>
       <c r="E52" s="5"/>
       <c r="G52" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H52" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I52" s="1">
@@ -1788,11 +1878,11 @@
       <c r="D53" s="4"/>
       <c r="E53" s="5"/>
       <c r="G53" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H53" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I53" s="1">
@@ -1806,11 +1896,11 @@
       <c r="D54" s="4"/>
       <c r="E54" s="5"/>
       <c r="G54" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H54" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I54" s="1">
@@ -1824,11 +1914,11 @@
       <c r="D55" s="4"/>
       <c r="E55" s="5"/>
       <c r="G55" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H55" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I55" s="1">
@@ -1842,11 +1932,11 @@
       <c r="D56" s="4"/>
       <c r="E56" s="5"/>
       <c r="G56" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H56" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I56" s="1">
@@ -1860,11 +1950,11 @@
       <c r="D57" s="4"/>
       <c r="E57" s="5"/>
       <c r="G57" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H57" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I57" s="1">
@@ -1878,11 +1968,11 @@
       <c r="D58" s="4"/>
       <c r="E58" s="5"/>
       <c r="G58" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H58" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I58" s="1">
@@ -1896,11 +1986,11 @@
       <c r="D59" s="4"/>
       <c r="E59" s="5"/>
       <c r="G59" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H59" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I59" s="1">
@@ -1911,11 +2001,11 @@
     <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60" s="4"/>
       <c r="G60" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H60" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I60" s="1">
@@ -1926,11 +2016,11 @@
     <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
       <c r="G61" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H61" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I61" s="1">
@@ -1941,11 +2031,11 @@
     <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B62" s="4"/>
       <c r="G62" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H62" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I62" s="1">
@@ -1956,11 +2046,11 @@
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="4"/>
       <c r="G63" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H63" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I63" s="1">
@@ -1971,11 +2061,11 @@
     <row r="64" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B64" s="4"/>
       <c r="G64" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H64" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I64" s="1">
@@ -2033,7 +2123,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G67" s="6" t="str">
-        <f t="shared" ref="G67:G98" si="5">IF(I67&gt;0,I67,IF(I67=0, " ", "ERROR"))</f>
+        <f t="shared" ref="G67:G98" si="7">IF(I67&gt;0,I67,IF(I67=0, " ", "ERROR"))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H67" s="1" t="str">
@@ -2047,11 +2137,11 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G68" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H68" s="1" t="str">
-        <f t="shared" ref="H68:H98" si="6">IF(AND(G68&lt;&gt;" ",G68&lt;&gt;"ERROR",H67&lt;&gt;" ", H67&lt;&gt;"ERROR"),G68+H67," ")</f>
+        <f t="shared" ref="H68:H98" si="8">IF(AND(G68&lt;&gt;" ",G68&lt;&gt;"ERROR",H67&lt;&gt;" ", H67&lt;&gt;"ERROR"),G68+H67," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I68" s="1">
@@ -2061,421 +2151,421 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G69" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H69" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I69" s="1">
-        <f t="shared" ref="I69:I132" si="7">((D69+E69)-(B69+C69))*24</f>
+        <f t="shared" ref="I69:I132" si="9">((D69+E69)-(B69+C69))*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G70" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H70" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I70" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G71" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H71" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I71" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G72" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H72" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I72" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G73" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H73" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I73" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G74" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H74" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I74" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G75" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H75" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I75" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G76" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H76" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I76" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G77" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H77" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I77" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G78" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H78" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I78" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G79" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H79" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I79" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G80" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H80" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I80" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G81" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H81" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I81" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G82" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H82" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I82" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G83" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H83" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I83" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G84" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H84" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I84" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G85" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H85" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I85" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G86" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H86" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I86" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G87" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H87" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I87" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G88" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H88" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I88" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G89" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H89" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I89" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G90" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H90" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I90" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G91" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H91" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I91" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G92" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H92" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I92" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G93" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H93" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I93" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G94" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H94" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I94" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G95" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H95" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I95" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G96" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H96" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I96" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G97" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H97" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I97" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G98" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H98" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I98" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2501,7 +2591,7 @@
         <v>6</v>
       </c>
       <c r="I99" s="1" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2523,13 +2613,13 @@
       <c r="G100" s="7"/>
       <c r="H100" s="7"/>
       <c r="I100" s="1" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G101" s="6" t="str">
-        <f t="shared" ref="G101:G132" si="8">IF(I101&gt;0,I101,IF(I101=0, " ", "ERROR"))</f>
+        <f t="shared" ref="G101:G132" si="10">IF(I101&gt;0,I101,IF(I101=0, " ", "ERROR"))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H101" s="1" t="str">
@@ -2537,441 +2627,441 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I101" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G102" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H102" s="1" t="str">
-        <f t="shared" ref="H102:H132" si="9">IF(AND(G102&lt;&gt;" ",G102&lt;&gt;"ERROR",H101&lt;&gt;" ", H101&lt;&gt;"ERROR"),G102+H101," ")</f>
+        <f t="shared" ref="H102:H132" si="11">IF(AND(G102&lt;&gt;" ",G102&lt;&gt;"ERROR",H101&lt;&gt;" ", H101&lt;&gt;"ERROR"),G102+H101," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I102" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G103" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H103" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I103" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G104" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H104" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I104" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G105" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H105" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I105" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G106" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H106" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I106" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G107" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H107" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I107" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G108" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H108" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I108" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G109" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H109" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I109" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G110" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H110" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I110" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G111" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H111" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I111" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G112" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H112" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I112" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G113" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H113" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I113" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G114" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H114" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I114" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G115" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H115" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I115" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G116" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H116" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I116" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G117" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H117" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I117" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G118" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H118" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I118" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G119" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H119" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I119" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G120" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H120" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I120" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G121" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H121" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I121" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G122" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H122" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I122" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G123" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H123" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I123" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G124" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H124" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I124" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G125" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H125" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I125" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G126" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H126" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I126" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G127" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H127" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I127" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G128" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H128" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I128" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G129" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H129" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I129" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G130" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H130" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I130" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G131" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H131" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I131" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G132" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H132" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I132" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>